<commit_message>
sql injection and port scanning
</commit_message>
<xml_diff>
--- a/traffic_data.xlsx
+++ b/traffic_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itay.talias/Private/BIU/SOC-algorithm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBDD030-816E-DA45-9B0C-0DF0F3E9767B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57184E36-717B-EA42-BAFC-59247FB779AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4400" yWindow="2500" windowWidth="28040" windowHeight="17440" xr2:uid="{E71518B3-EFFA-D744-A651-3772FD64B2FC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>source_ip</t>
   </si>
@@ -59,23 +59,32 @@
     <t>2.2.2.2</t>
   </si>
   <si>
-    <t>sasdfsd</t>
-  </si>
-  <si>
-    <t>safsf</t>
-  </si>
-  <si>
     <t>4.4.4.4</t>
   </si>
   <si>
     <t>line</t>
+  </si>
+  <si>
+    <t>1.2.3.4</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>itay</t>
+  </si>
+  <si>
+    <t>itay1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,6 +107,13 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,10 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379D3C87-89C1-7446-8F27-B26EC4E4013A}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,8 +488,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
+      <c r="A1" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -494,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -505,8 +523,8 @@
       <c r="E2">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -525,11 +543,52 @@
       <c r="E3">
         <v>80</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="E5">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>